<commit_message>
updating with new Files for Faculty Module
</commit_message>
<xml_diff>
--- a/Module Assignment.xlsx
+++ b/Module Assignment.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Jordan\Software Engineering Thesis Files\Drop Here\Mother Of Perpetual Help\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Acer\Documents\NetBeansProjects\MphsEnrollmentSystem\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -284,7 +284,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="54">
+  <dxfs count="10">
     <dxf>
       <fill>
         <patternFill>
@@ -341,365 +341,6 @@
       <fill>
         <patternFill>
           <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF0070C0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF0070C0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF0070C0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF0070C0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1002,7 +643,7 @@
   <dimension ref="A1:Q31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1111,7 +752,7 @@
         <v>22</v>
       </c>
       <c r="B8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C8" s="4">
         <v>0</v>

</xml_diff>